<commit_message>
updating the weekly logs for myself
</commit_message>
<xml_diff>
--- a/Class Documents/User Information/GadaletaJakeWeeklogs.xlsx
+++ b/Class Documents/User Information/GadaletaJakeWeeklogs.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Week 1" sheetId="1" state="visible" r:id="rId2"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="53">
   <si>
     <t xml:space="preserve">Items</t>
   </si>
@@ -138,6 +138,67 @@
 2. Wrote the backend server information and handled the bundling
 3. Wrote the code checker in such a way that it always returns in native HTML
 4. Looked into pytests and github actions to see if we could automate some testing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Requirement</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Index: Build the URL, link HTML, CSS, &amp; JavaScript </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Time Expected Time</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Expected Time</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Actual Time</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Short Description</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Linked the foder code to render is flask bundled the appropriate CSS &amp; JS files in such a way that they are easily comparable</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dif from what was expected</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The decision was made to “Hyper Load” the bundling process speed up load times by 22% (this applies to the other similar work items)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Student: Build the URL, link HTML, CSS, &amp; JavaScript </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Teacher: Build the URL, link HTML, CSS, &amp; JavaScript </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Interviewer: Build the URL, link HTML, CSS, &amp; JavaScript </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Interviewee: Build the URL, link HTML, CSS, &amp; JavaScript </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Backend: Text Comparison Code, written in
+python and rust (as a backup)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Additional Issues 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Getting everyone setup</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The others had a hard time setting up their environments to try to automate the process a little I used a lot of scripting .bat, .py, .shs you name it we got it</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Additional Issues 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Flask / Jinga fighting with nick on the front end</t>
+  </si>
+  <si>
+    <t xml:space="preserve">For about a day nick was stuck waiting for me to get some flask stuff together, the issues were highly unexpected and hence took very long to fix</t>
   </si>
   <si>
     <t xml:space="preserve">1.
@@ -159,7 +220,6 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -181,22 +241,26 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="16"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF000000"/>
+        <bgColor rgb="FF003300"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -240,7 +304,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -273,6 +337,14 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -296,9 +368,9 @@
       <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
-    <row r="1" s="2" customFormat="true" ht="19" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" s="2" customFormat="true" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -329,7 +401,7 @@
       <c r="X1" s="1"/>
       <c r="Y1" s="1"/>
     </row>
-    <row r="2" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
         <v>2</v>
       </c>
@@ -360,7 +432,7 @@
       <c r="X2" s="4"/>
       <c r="Y2" s="4"/>
     </row>
-    <row r="3" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
         <v>4</v>
       </c>
@@ -391,7 +463,7 @@
       <c r="X3" s="4"/>
       <c r="Y3" s="4"/>
     </row>
-    <row r="4" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
         <v>6</v>
       </c>
@@ -484,7 +556,7 @@
       <c r="X6" s="7"/>
       <c r="Y6" s="7"/>
     </row>
-    <row r="7" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="s">
         <v>12</v>
       </c>
@@ -553,9 +625,12 @@
       <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="64" min="1" style="0" width="8.67"/>
+  </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="19" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -586,7 +661,7 @@
       <c r="X1" s="1"/>
       <c r="Y1" s="1"/>
     </row>
-    <row r="2" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
         <v>2</v>
       </c>
@@ -615,7 +690,7 @@
       <c r="X2" s="4"/>
       <c r="Y2" s="4"/>
     </row>
-    <row r="3" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
         <v>4</v>
       </c>
@@ -644,7 +719,7 @@
       <c r="X3" s="4"/>
       <c r="Y3" s="4"/>
     </row>
-    <row r="4" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
         <v>6</v>
       </c>
@@ -719,7 +794,7 @@
       <c r="L6" s="6"/>
       <c r="M6" s="6"/>
       <c r="N6" s="7" t="s">
-        <v>32</v>
+        <v>52</v>
       </c>
       <c r="O6" s="7"/>
       <c r="P6" s="7"/>
@@ -733,7 +808,7 @@
       <c r="X6" s="7"/>
       <c r="Y6" s="7"/>
     </row>
-    <row r="7" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="s">
         <v>12</v>
       </c>
@@ -800,9 +875,12 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="64" min="1" style="0" width="8.67"/>
+  </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="19" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -833,7 +911,7 @@
       <c r="X1" s="1"/>
       <c r="Y1" s="1"/>
     </row>
-    <row r="2" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
         <v>2</v>
       </c>
@@ -864,7 +942,7 @@
       <c r="X2" s="4"/>
       <c r="Y2" s="4"/>
     </row>
-    <row r="3" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
         <v>4</v>
       </c>
@@ -895,7 +973,7 @@
       <c r="X3" s="4"/>
       <c r="Y3" s="4"/>
     </row>
-    <row r="4" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
         <v>6</v>
       </c>
@@ -988,7 +1066,7 @@
       <c r="X6" s="7"/>
       <c r="Y6" s="7"/>
     </row>
-    <row r="7" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="s">
         <v>12</v>
       </c>
@@ -1057,9 +1135,12 @@
       <selection pane="topLeft" activeCell="N8" activeCellId="0" sqref="N8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="64" min="1" style="0" width="8.67"/>
+  </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="19" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1090,7 +1171,7 @@
       <c r="X1" s="1"/>
       <c r="Y1" s="1"/>
     </row>
-    <row r="2" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
         <v>2</v>
       </c>
@@ -1121,7 +1202,7 @@
       <c r="X2" s="4"/>
       <c r="Y2" s="4"/>
     </row>
-    <row r="3" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
         <v>4</v>
       </c>
@@ -1152,7 +1233,7 @@
       <c r="X3" s="4"/>
       <c r="Y3" s="4"/>
     </row>
-    <row r="4" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
         <v>6</v>
       </c>
@@ -1245,7 +1326,7 @@
       <c r="X6" s="7"/>
       <c r="Y6" s="7"/>
     </row>
-    <row r="7" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="s">
         <v>12</v>
       </c>
@@ -1314,9 +1395,12 @@
       <selection pane="topLeft" activeCell="N8" activeCellId="0" sqref="N8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="64" min="1" style="0" width="8.67"/>
+  </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="19" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1347,7 +1431,7 @@
       <c r="X1" s="1"/>
       <c r="Y1" s="1"/>
     </row>
-    <row r="2" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
         <v>2</v>
       </c>
@@ -1378,7 +1462,7 @@
       <c r="X2" s="4"/>
       <c r="Y2" s="4"/>
     </row>
-    <row r="3" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
         <v>4</v>
       </c>
@@ -1409,7 +1493,7 @@
       <c r="X3" s="4"/>
       <c r="Y3" s="4"/>
     </row>
-    <row r="4" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
         <v>6</v>
       </c>
@@ -1502,7 +1586,7 @@
       <c r="X6" s="7"/>
       <c r="Y6" s="7"/>
     </row>
-    <row r="7" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="s">
         <v>12</v>
       </c>
@@ -1571,9 +1655,12 @@
       <selection pane="topLeft" activeCell="N8" activeCellId="0" sqref="N8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="64" min="1" style="0" width="8.67"/>
+  </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="19" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1604,7 +1691,7 @@
       <c r="X1" s="1"/>
       <c r="Y1" s="1"/>
     </row>
-    <row r="2" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
         <v>2</v>
       </c>
@@ -1635,7 +1722,7 @@
       <c r="X2" s="4"/>
       <c r="Y2" s="4"/>
     </row>
-    <row r="3" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
         <v>4</v>
       </c>
@@ -1666,7 +1753,7 @@
       <c r="X3" s="4"/>
       <c r="Y3" s="4"/>
     </row>
-    <row r="4" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
         <v>6</v>
       </c>
@@ -1759,7 +1846,7 @@
       <c r="X6" s="7"/>
       <c r="Y6" s="7"/>
     </row>
-    <row r="7" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="s">
         <v>12</v>
       </c>
@@ -1824,13 +1911,16 @@
   </sheetPr>
   <dimension ref="A1:Y7"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="N8" activeCellId="0" sqref="N8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="64" min="1" style="0" width="8.67"/>
+  </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="19" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1861,7 +1951,7 @@
       <c r="X1" s="1"/>
       <c r="Y1" s="1"/>
     </row>
-    <row r="2" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
         <v>2</v>
       </c>
@@ -1892,7 +1982,7 @@
       <c r="X2" s="4"/>
       <c r="Y2" s="4"/>
     </row>
-    <row r="3" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
         <v>4</v>
       </c>
@@ -1923,7 +2013,7 @@
       <c r="X3" s="4"/>
       <c r="Y3" s="4"/>
     </row>
-    <row r="4" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
         <v>6</v>
       </c>
@@ -2016,7 +2106,7 @@
       <c r="X6" s="7"/>
       <c r="Y6" s="7"/>
     </row>
-    <row r="7" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="s">
         <v>12</v>
       </c>
@@ -2080,238 +2170,329 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A16:Y22"/>
+  <dimension ref="A1:E43"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A21" activeCellId="0" sqref="A21"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D4" activeCellId="0" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="24.91"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="120.77"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="8.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="12.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="64" min="5" style="0" width="8.67"/>
+  </cols>
   <sheetData>
-    <row r="16" customFormat="false" ht="19" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B16" s="1"/>
-      <c r="C16" s="1"/>
-      <c r="D16" s="1"/>
-      <c r="E16" s="1"/>
-      <c r="F16" s="1"/>
-      <c r="G16" s="1"/>
-      <c r="H16" s="1"/>
-      <c r="I16" s="1"/>
-      <c r="J16" s="1"/>
-      <c r="K16" s="1"/>
-      <c r="L16" s="1"/>
-      <c r="M16" s="1"/>
-      <c r="N16" s="1" t="s">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="B2" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="O16" s="1"/>
-      <c r="P16" s="1"/>
-      <c r="Q16" s="1"/>
-      <c r="R16" s="1"/>
-      <c r="S16" s="1"/>
-      <c r="T16" s="1"/>
-      <c r="U16" s="1"/>
-      <c r="V16" s="1"/>
-      <c r="W16" s="1"/>
-      <c r="X16" s="1"/>
-      <c r="Y16" s="1"/>
-    </row>
-    <row r="17" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="3" t="s">
+      <c r="D2" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="E2" s="0" t="n">
+        <f aca="false">B2 + B8 + B14 + B20 + B26 + B32</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="B3" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="E3" s="0" t="n">
+        <f aca="false">B3 + B9 + B15 + B21 + B27 + B33 + B38 + B42</f>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="8"/>
+      <c r="B6" s="8"/>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="B8" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="B9" s="0" t="n">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="B10" s="0" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="8"/>
+      <c r="B12" s="8"/>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="B13" s="0" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="B14" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="B15" s="0" t="n">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="B16" s="0" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="8"/>
+      <c r="B18" s="8"/>
+    </row>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="B19" s="0" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="B20" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="B21" s="0" t="n">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="B22" s="0" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="0" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="8"/>
+      <c r="B24" s="8"/>
+    </row>
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="B25" s="0" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="B26" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="B27" s="0" t="n">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="B28" s="0" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="0" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="8"/>
+      <c r="B30" s="8"/>
+    </row>
+    <row r="31" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="B31" s="9" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="B32" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="B17" s="3"/>
-      <c r="C17" s="3"/>
-      <c r="D17" s="3"/>
-      <c r="E17" s="3"/>
-      <c r="F17" s="3"/>
-      <c r="G17" s="3"/>
-      <c r="H17" s="3"/>
-      <c r="I17" s="3"/>
-      <c r="J17" s="3"/>
-      <c r="K17" s="3"/>
-      <c r="L17" s="3"/>
-      <c r="M17" s="3"/>
-      <c r="N17" s="4"/>
-      <c r="O17" s="4"/>
-      <c r="P17" s="4"/>
-      <c r="Q17" s="4"/>
-      <c r="R17" s="4"/>
-      <c r="S17" s="4"/>
-      <c r="T17" s="4"/>
-      <c r="U17" s="4"/>
-      <c r="V17" s="4"/>
-      <c r="W17" s="4"/>
-      <c r="X17" s="4"/>
-      <c r="Y17" s="4"/>
-    </row>
-    <row r="18" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B18" s="3"/>
-      <c r="C18" s="3"/>
-      <c r="D18" s="3"/>
-      <c r="E18" s="3"/>
-      <c r="F18" s="3"/>
-      <c r="G18" s="3"/>
-      <c r="H18" s="3"/>
-      <c r="I18" s="3"/>
-      <c r="J18" s="3"/>
-      <c r="K18" s="3"/>
-      <c r="L18" s="3"/>
-      <c r="M18" s="3"/>
-      <c r="N18" s="4"/>
-      <c r="O18" s="4"/>
-      <c r="P18" s="4"/>
-      <c r="Q18" s="4"/>
-      <c r="R18" s="4"/>
-      <c r="S18" s="4"/>
-      <c r="T18" s="4"/>
-      <c r="U18" s="4"/>
-      <c r="V18" s="4"/>
-      <c r="W18" s="4"/>
-      <c r="X18" s="4"/>
-      <c r="Y18" s="4"/>
-    </row>
-    <row r="19" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B19" s="3"/>
-      <c r="C19" s="3"/>
-      <c r="D19" s="3"/>
-      <c r="E19" s="3"/>
-      <c r="F19" s="3"/>
-      <c r="G19" s="3"/>
-      <c r="H19" s="3"/>
-      <c r="I19" s="3"/>
-      <c r="J19" s="3"/>
-      <c r="K19" s="3"/>
-      <c r="L19" s="3"/>
-      <c r="M19" s="3"/>
-      <c r="N19" s="4"/>
-      <c r="O19" s="4"/>
-      <c r="P19" s="4"/>
-      <c r="Q19" s="4"/>
-      <c r="R19" s="4"/>
-      <c r="S19" s="4"/>
-      <c r="T19" s="4"/>
-      <c r="U19" s="4"/>
-      <c r="V19" s="4"/>
-      <c r="W19" s="4"/>
-      <c r="X19" s="4"/>
-      <c r="Y19" s="4"/>
-    </row>
-    <row r="20" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A20" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B20" s="5"/>
-      <c r="C20" s="5"/>
-      <c r="D20" s="5"/>
-      <c r="E20" s="5"/>
-      <c r="F20" s="5"/>
-      <c r="G20" s="5"/>
-      <c r="H20" s="5"/>
-      <c r="I20" s="5"/>
-      <c r="J20" s="5"/>
-      <c r="K20" s="5"/>
-      <c r="L20" s="5"/>
-      <c r="M20" s="5"/>
-      <c r="N20" s="4"/>
-      <c r="O20" s="4"/>
-      <c r="P20" s="4"/>
-      <c r="Q20" s="4"/>
-      <c r="R20" s="4"/>
-      <c r="S20" s="4"/>
-      <c r="T20" s="4"/>
-      <c r="U20" s="4"/>
-      <c r="V20" s="4"/>
-      <c r="W20" s="4"/>
-      <c r="X20" s="4"/>
-      <c r="Y20" s="4"/>
-    </row>
-    <row r="21" customFormat="false" ht="162" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A21" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="B21" s="6"/>
-      <c r="C21" s="6"/>
-      <c r="D21" s="6"/>
-      <c r="E21" s="6"/>
-      <c r="F21" s="6"/>
-      <c r="G21" s="6"/>
-      <c r="H21" s="6"/>
-      <c r="I21" s="6"/>
-      <c r="J21" s="6"/>
-      <c r="K21" s="6"/>
-      <c r="L21" s="6"/>
-      <c r="M21" s="6"/>
-      <c r="N21" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="O21" s="7"/>
-      <c r="P21" s="7"/>
-      <c r="Q21" s="7"/>
-      <c r="R21" s="7"/>
-      <c r="S21" s="7"/>
-      <c r="T21" s="7"/>
-      <c r="U21" s="7"/>
-      <c r="V21" s="7"/>
-      <c r="W21" s="7"/>
-      <c r="X21" s="7"/>
-      <c r="Y21" s="7"/>
-    </row>
-    <row r="22" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B22" s="3"/>
-      <c r="C22" s="3"/>
-      <c r="D22" s="3"/>
-      <c r="E22" s="3"/>
-      <c r="F22" s="3"/>
-      <c r="G22" s="3"/>
-      <c r="H22" s="3"/>
-      <c r="I22" s="3"/>
-      <c r="J22" s="3"/>
-      <c r="K22" s="3"/>
-      <c r="L22" s="3"/>
-      <c r="M22" s="3"/>
-      <c r="N22" s="4"/>
-      <c r="O22" s="4"/>
-      <c r="P22" s="4"/>
-      <c r="Q22" s="4"/>
-      <c r="R22" s="4"/>
-      <c r="S22" s="4"/>
-      <c r="T22" s="4"/>
-      <c r="U22" s="4"/>
-      <c r="V22" s="4"/>
-      <c r="W22" s="4"/>
-      <c r="X22" s="4"/>
-      <c r="Y22" s="4"/>
+    </row>
+    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="B33" s="0" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="B34" s="0" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="0" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="B37" s="0" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="B38" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="B39" s="0" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="B41" s="0" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="B42" s="0" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="B43" s="0" t="s">
+        <v>51</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="14">
-    <mergeCell ref="A16:M16"/>
-    <mergeCell ref="N16:Y16"/>
-    <mergeCell ref="A17:M17"/>
-    <mergeCell ref="N17:Y17"/>
-    <mergeCell ref="A18:M18"/>
-    <mergeCell ref="N18:Y18"/>
-    <mergeCell ref="A19:M19"/>
-    <mergeCell ref="N19:Y19"/>
-    <mergeCell ref="A20:M20"/>
-    <mergeCell ref="N20:Y20"/>
-    <mergeCell ref="A21:M21"/>
-    <mergeCell ref="N21:Y21"/>
-    <mergeCell ref="A22:M22"/>
-    <mergeCell ref="N22:Y22"/>
-  </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -2333,9 +2514,12 @@
       <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="64" min="1" style="0" width="8.67"/>
+  </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="19" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2366,7 +2550,7 @@
       <c r="X1" s="1"/>
       <c r="Y1" s="1"/>
     </row>
-    <row r="2" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
         <v>2</v>
       </c>
@@ -2395,7 +2579,7 @@
       <c r="X2" s="4"/>
       <c r="Y2" s="4"/>
     </row>
-    <row r="3" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
         <v>4</v>
       </c>
@@ -2424,7 +2608,7 @@
       <c r="X3" s="4"/>
       <c r="Y3" s="4"/>
     </row>
-    <row r="4" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
         <v>6</v>
       </c>
@@ -2499,7 +2683,7 @@
       <c r="L6" s="6"/>
       <c r="M6" s="6"/>
       <c r="N6" s="7" t="s">
-        <v>32</v>
+        <v>52</v>
       </c>
       <c r="O6" s="7"/>
       <c r="P6" s="7"/>
@@ -2513,7 +2697,7 @@
       <c r="X6" s="7"/>
       <c r="Y6" s="7"/>
     </row>
-    <row r="7" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="s">
         <v>12</v>
       </c>
@@ -2580,9 +2764,12 @@
       <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="64" min="1" style="0" width="8.67"/>
+  </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="19" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2613,7 +2800,7 @@
       <c r="X1" s="1"/>
       <c r="Y1" s="1"/>
     </row>
-    <row r="2" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
         <v>2</v>
       </c>
@@ -2642,7 +2829,7 @@
       <c r="X2" s="4"/>
       <c r="Y2" s="4"/>
     </row>
-    <row r="3" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
         <v>4</v>
       </c>
@@ -2671,7 +2858,7 @@
       <c r="X3" s="4"/>
       <c r="Y3" s="4"/>
     </row>
-    <row r="4" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
         <v>6</v>
       </c>
@@ -2746,7 +2933,7 @@
       <c r="L6" s="6"/>
       <c r="M6" s="6"/>
       <c r="N6" s="7" t="s">
-        <v>32</v>
+        <v>52</v>
       </c>
       <c r="O6" s="7"/>
       <c r="P6" s="7"/>
@@ -2760,7 +2947,7 @@
       <c r="X6" s="7"/>
       <c r="Y6" s="7"/>
     </row>
-    <row r="7" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="s">
         <v>12</v>
       </c>
@@ -2827,9 +3014,12 @@
       <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="64" min="1" style="0" width="8.67"/>
+  </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="19" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2860,7 +3050,7 @@
       <c r="X1" s="1"/>
       <c r="Y1" s="1"/>
     </row>
-    <row r="2" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
         <v>2</v>
       </c>
@@ -2889,7 +3079,7 @@
       <c r="X2" s="4"/>
       <c r="Y2" s="4"/>
     </row>
-    <row r="3" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
         <v>4</v>
       </c>
@@ -2918,7 +3108,7 @@
       <c r="X3" s="4"/>
       <c r="Y3" s="4"/>
     </row>
-    <row r="4" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
         <v>6</v>
       </c>
@@ -2993,7 +3183,7 @@
       <c r="L6" s="6"/>
       <c r="M6" s="6"/>
       <c r="N6" s="7" t="s">
-        <v>32</v>
+        <v>52</v>
       </c>
       <c r="O6" s="7"/>
       <c r="P6" s="7"/>
@@ -3007,7 +3197,7 @@
       <c r="X6" s="7"/>
       <c r="Y6" s="7"/>
     </row>
-    <row r="7" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="s">
         <v>12</v>
       </c>

</xml_diff>